<commit_message>
before changing excel structure
</commit_message>
<xml_diff>
--- a/zOther Stuff/excels/result-upload-sample.xlsx
+++ b/zOther Stuff/excels/result-upload-sample.xlsx
@@ -49,7 +49,7 @@
     <t>02110113</t>
   </si>
   <si>
-    <t>02260113</t>
+    <t>02110114</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>